<commit_message>
OPTIMIZACION DE INTERFAZ NO.4
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/LOGGIN.xlsx
+++ b/ProyectoPooDist/excels/LOGGIN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseg\Downloads\PROYECTO CINDY\Proyecto-Poo-Dist\ProyectoPooDist\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17ADC7C0-2C20-44CE-9463-AC5E9024AACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E474F5B-1B70-4A11-940B-F18F2DB27125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="236">
   <si>
     <t>Tiempo Entrada</t>
   </si>
@@ -656,6 +656,78 @@
   </si>
   <si>
     <t>20/10/2024 00:20:03</t>
+  </si>
+  <si>
+    <t>20/10/2024 17:43:05</t>
+  </si>
+  <si>
+    <t>20/10/2024 17:43:12</t>
+  </si>
+  <si>
+    <t>20/10/2024 10:31:19</t>
+  </si>
+  <si>
+    <t>20/10/2024 10:32:42</t>
+  </si>
+  <si>
+    <t>20/10/2024 14:14:55</t>
+  </si>
+  <si>
+    <t>20/10/2024 14:14:58</t>
+  </si>
+  <si>
+    <t>20/10/2024 14:37:00</t>
+  </si>
+  <si>
+    <t>20/10/2024 14:40:07</t>
+  </si>
+  <si>
+    <t>20/10/2024 14:40:24</t>
+  </si>
+  <si>
+    <t>20/10/2024 14:41:48</t>
+  </si>
+  <si>
+    <t>20/10/2024 14:42:04</t>
+  </si>
+  <si>
+    <t>20/10/2024 14:49:01</t>
+  </si>
+  <si>
+    <t>20/10/2024 14:53:44</t>
+  </si>
+  <si>
+    <t>20/10/2024 14:54:10</t>
+  </si>
+  <si>
+    <t>20/10/2024 14:57:54</t>
+  </si>
+  <si>
+    <t>20/10/2024 15:49:58</t>
+  </si>
+  <si>
+    <t>20/10/2024 14:58:00</t>
+  </si>
+  <si>
+    <t>20/10/2024 17:33:23</t>
+  </si>
+  <si>
+    <t>20/10/2024 14:58:01</t>
+  </si>
+  <si>
+    <t>20/10/2024 17:35:56</t>
+  </si>
+  <si>
+    <t>20/10/2024 17:42:29</t>
+  </si>
+  <si>
+    <t>20/10/2024 17:42:34</t>
+  </si>
+  <si>
+    <t>20/10/2024 17:42:43</t>
+  </si>
+  <si>
+    <t>20/10/2024 17:42:55</t>
   </si>
 </sst>
 </file>
@@ -1031,10 +1103,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D106"/>
+  <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="C106" sqref="C106:C119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2523,6 +2595,188 @@
         <v>7</v>
       </c>
     </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C107" t="s">
+        <v>10</v>
+      </c>
+      <c r="D107" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C108" t="s">
+        <v>10</v>
+      </c>
+      <c r="D108" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C109" t="s">
+        <v>10</v>
+      </c>
+      <c r="D109" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C110" t="s">
+        <v>10</v>
+      </c>
+      <c r="D110" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C111" t="s">
+        <v>10</v>
+      </c>
+      <c r="D111" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C112" t="s">
+        <v>10</v>
+      </c>
+      <c r="D112" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C113" t="s">
+        <v>10</v>
+      </c>
+      <c r="D113" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C114" t="s">
+        <v>10</v>
+      </c>
+      <c r="D114" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C115" t="s">
+        <v>10</v>
+      </c>
+      <c r="D115" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C116" t="s">
+        <v>10</v>
+      </c>
+      <c r="D116" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C117" t="s">
+        <v>10</v>
+      </c>
+      <c r="D117" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C118" t="s">
+        <v>10</v>
+      </c>
+      <c r="D118" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C119" t="s">
+        <v>10</v>
+      </c>
+      <c r="D119" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
OPTIMIZACION DE DISEÑO NO.7
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/LOGGIN.xlsx
+++ b/ProyectoPooDist/excels/LOGGIN.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="557">
   <si>
     <t>Tiempo Entrada</t>
   </si>
@@ -722,927 +722,933 @@
     <t>20/10/2024 17:42:55</t>
   </si>
   <si>
+    <t>22/10/2024 00:16:01</t>
+  </si>
+  <si>
+    <t>22/10/2024 01:39:19</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>21/10/2024 06:19:20</t>
+  </si>
+  <si>
+    <t>21/10/2024 06:20:32</t>
+  </si>
+  <si>
+    <t>21/10/2024 06:29:18</t>
+  </si>
+  <si>
+    <t>21/10/2024 06:30:52</t>
+  </si>
+  <si>
+    <t>21/10/2024 06:50:12</t>
+  </si>
+  <si>
+    <t>21/10/2024 06:51:02</t>
+  </si>
+  <si>
+    <t>21/10/2024 06:51:46</t>
+  </si>
+  <si>
+    <t>21/10/2024 06:52:35</t>
+  </si>
+  <si>
+    <t>21/10/2024 07:55:32</t>
+  </si>
+  <si>
+    <t>21/10/2024 07:56:34</t>
+  </si>
+  <si>
+    <t>21/10/2024 08:21:11</t>
+  </si>
+  <si>
+    <t>21/10/2024 08:26:04</t>
+  </si>
+  <si>
+    <t>21/10/2024 08:22:37</t>
+  </si>
+  <si>
+    <t>21/10/2024 08:30:58</t>
+  </si>
+  <si>
+    <t>21/10/2024 08:25:17</t>
+  </si>
+  <si>
+    <t>21/10/2024 18:51:53</t>
+  </si>
+  <si>
+    <t>21/10/2024 08:26:24</t>
+  </si>
+  <si>
+    <t>21/10/2024 18:51:54</t>
+  </si>
+  <si>
+    <t>21/10/2024 08:28:36</t>
+  </si>
+  <si>
+    <t>21/10/2024 19:28:58</t>
+  </si>
+  <si>
+    <t>21/10/2024 08:32:33</t>
+  </si>
+  <si>
+    <t>21/10/2024 19:31:36</t>
+  </si>
+  <si>
+    <t>21/10/2024 08:35:11</t>
+  </si>
+  <si>
+    <t>21/10/2024 19:33:13</t>
+  </si>
+  <si>
+    <t>21/10/2024 18:51:42</t>
+  </si>
+  <si>
+    <t>21/10/2024 19:39:01</t>
+  </si>
+  <si>
+    <t>21/10/2024 19:30:29</t>
+  </si>
+  <si>
+    <t>21/10/2024 19:45:27</t>
+  </si>
+  <si>
+    <t>21/10/2024 19:31:56</t>
+  </si>
+  <si>
+    <t>21/10/2024 20:24:36</t>
+  </si>
+  <si>
+    <t>21/10/2024 19:35:20</t>
+  </si>
+  <si>
+    <t>21/10/2024 20:25:20</t>
+  </si>
+  <si>
+    <t>21/10/2024 19:39:13</t>
+  </si>
+  <si>
+    <t>21/10/2024 20:26:27</t>
+  </si>
+  <si>
+    <t>21/10/2024 20:19:17</t>
+  </si>
+  <si>
+    <t>21/10/2024 20:42:29</t>
+  </si>
+  <si>
+    <t>21/10/2024 20:20:27</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:13:00</t>
+  </si>
+  <si>
+    <t>21/10/2024 20:21:24</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:15:05</t>
+  </si>
+  <si>
+    <t>21/10/2024 20:22:31</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:16:31</t>
+  </si>
+  <si>
+    <t>21/10/2024 20:24:52</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:22:27</t>
+  </si>
+  <si>
+    <t>21/10/2024 20:25:38</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:29:16</t>
+  </si>
+  <si>
+    <t>21/10/2024 20:41:49</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:31:20</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:10:56</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:39:02</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:13:26</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:46:00</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:15:30</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:49:29</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:21:50</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:49:31</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:23:10</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:51:46</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:27:49</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:52:46</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:27:51</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:53:30</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:29:55</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:54:03</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:35:01</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:55:01</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:45:13</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:55:25</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:46:17</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:56:07</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:49:07</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:56:41</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:49:45</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:57:02</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:52:04</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:58:16</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:53:03</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:59:35</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:53:46</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:00:57</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:54:18</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:01:29</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:55:09</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:01:50</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:55:42</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:02:08</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:55:43</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:02:36</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:56:26</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:03:12</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:58:00</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:07:02</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:58:32</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:10:42</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:59:53</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:12:00</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:01:11</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:12:03</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:01:32</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:13:21</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:02:03</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:13:57</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:02:11</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:15:01</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:02:51</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:15:25</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:03:25</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:18:46</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:10:13</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:21:11</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:10:14</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:22:04</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:11:00</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:22:47</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:12:19</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:23:13</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:13:37</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:25:08</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:14:13</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:26:08</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:15:12</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:26:49</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:15:14</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:27:39</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:15:53</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:28:21</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:19:02</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:29:11</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:21:28</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:29:48</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:22:24</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:30:22</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:23:01</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:31:54</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:23:03</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:32:43</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:23:34</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:34:05</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:23:36</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:35:20</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:25:47</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:37:37</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:26:21</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:40:58</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:27:03</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:41:25</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:27:52</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:41:49</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:28:35</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:42:19</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:28:36</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:44:34</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:29:26</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:45:01</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:30:04</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:45:31</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:30:37</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:46:55</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:32:07</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:48:16</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:33:37</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:49:04</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:34:28</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:49:42</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:35:48</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:50:04</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:37:50</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:50:46</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:41:11</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:52:28</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:41:39</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:53:01</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:42:04</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:53:51</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:42:39</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:54:20</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:43:45</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:55:15</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:44:47</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:55:39</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:45:17</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:56:39</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:45:43</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:57:47</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:47:11</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:58:41</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:48:34</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:59:10</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:49:15</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:59:37</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:49:55</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:00:05</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:50:16</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:00:56</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:50:59</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:01:54</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:52:50</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:03:40</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:53:15</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:04:21</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:54:05</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:05:04</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:54:36</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:06:02</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:55:28</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:10:35</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:56:25</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:11:09</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:56:53</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:11:40</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:58:01</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:12:16</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:58:56</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:12:43</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:59:25</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:13:18</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:59:51</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:16:34</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:00:18</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:20:09</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:01:08</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:20:41</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:02:06</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:31:14</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:03:54</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:32:20</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:04:34</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:32:56</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:05:17</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:34:03</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:06:15</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:35:02</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:10:46</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:36:01</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:11:22</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:37:00</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:11:51</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:37:30</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:12:28</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:37:59</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:12:55</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:38:34</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:13:45</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:46:05</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:16:46</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:46:45</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:20:22</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:47:32</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:22:38</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:48:19</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:29:51</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:51:43</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:31:28</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:54:52</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:32:34</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:55:45</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:33:28</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:56:49</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:34:18</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:57:29</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:35:14</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:58:19</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:36:13</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:00:00</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:37:12</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:02:23</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:37:42</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:03:09</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:38:10</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:08:10</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:38:46</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:09:54</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:46:17</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:11:17</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:47:09</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:15:42</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:47:49</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:16:12</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:49:52</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:20:34</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:52:35</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:32:28</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:55:13</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:39:02</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:56:17</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:40:04</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:57:09</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:51:12</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:57:51</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:57:53</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:58:34</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:58:26</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:00:38</t>
+  </si>
+  <si>
+    <t>22/10/2024 01:10:53</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:02:59</t>
+  </si>
+  <si>
+    <t>22/10/2024 01:13:37</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:05:41</t>
+  </si>
+  <si>
+    <t>22/10/2024 01:15:46</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:08:29</t>
+  </si>
+  <si>
+    <t>22/10/2024 01:16:13</t>
+  </si>
+  <si>
     <t>22/10/2024 00:11:00</t>
   </si>
   <si>
     <t>22/10/2024 01:16:32</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>21/10/2024 06:19:20</t>
-  </si>
-  <si>
-    <t>21/10/2024 06:20:32</t>
-  </si>
-  <si>
-    <t>21/10/2024 06:29:18</t>
-  </si>
-  <si>
-    <t>21/10/2024 06:30:52</t>
-  </si>
-  <si>
-    <t>21/10/2024 06:50:12</t>
-  </si>
-  <si>
-    <t>21/10/2024 06:51:02</t>
-  </si>
-  <si>
-    <t>21/10/2024 06:51:46</t>
-  </si>
-  <si>
-    <t>21/10/2024 06:52:35</t>
-  </si>
-  <si>
-    <t>21/10/2024 07:55:32</t>
-  </si>
-  <si>
-    <t>21/10/2024 07:56:34</t>
-  </si>
-  <si>
-    <t>21/10/2024 08:21:11</t>
-  </si>
-  <si>
-    <t>21/10/2024 08:26:04</t>
-  </si>
-  <si>
-    <t>21/10/2024 08:22:37</t>
-  </si>
-  <si>
-    <t>21/10/2024 08:30:58</t>
-  </si>
-  <si>
-    <t>21/10/2024 08:25:17</t>
-  </si>
-  <si>
-    <t>21/10/2024 18:51:53</t>
-  </si>
-  <si>
-    <t>21/10/2024 08:26:24</t>
-  </si>
-  <si>
-    <t>21/10/2024 18:51:54</t>
-  </si>
-  <si>
-    <t>21/10/2024 08:28:36</t>
-  </si>
-  <si>
-    <t>21/10/2024 19:28:58</t>
-  </si>
-  <si>
-    <t>21/10/2024 08:32:33</t>
-  </si>
-  <si>
-    <t>21/10/2024 19:31:36</t>
-  </si>
-  <si>
-    <t>21/10/2024 08:35:11</t>
-  </si>
-  <si>
-    <t>21/10/2024 19:33:13</t>
-  </si>
-  <si>
-    <t>21/10/2024 18:51:42</t>
-  </si>
-  <si>
-    <t>21/10/2024 19:39:01</t>
-  </si>
-  <si>
-    <t>21/10/2024 19:30:29</t>
-  </si>
-  <si>
-    <t>21/10/2024 19:45:27</t>
-  </si>
-  <si>
-    <t>21/10/2024 19:31:56</t>
-  </si>
-  <si>
-    <t>21/10/2024 20:24:36</t>
-  </si>
-  <si>
-    <t>21/10/2024 19:35:20</t>
-  </si>
-  <si>
-    <t>21/10/2024 20:25:20</t>
-  </si>
-  <si>
-    <t>21/10/2024 19:39:13</t>
-  </si>
-  <si>
-    <t>21/10/2024 20:26:27</t>
-  </si>
-  <si>
-    <t>21/10/2024 20:19:17</t>
-  </si>
-  <si>
-    <t>21/10/2024 20:42:29</t>
-  </si>
-  <si>
-    <t>21/10/2024 20:20:27</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:13:00</t>
-  </si>
-  <si>
-    <t>21/10/2024 20:21:24</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:15:05</t>
-  </si>
-  <si>
-    <t>21/10/2024 20:22:31</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:16:31</t>
-  </si>
-  <si>
-    <t>21/10/2024 20:24:52</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:22:27</t>
-  </si>
-  <si>
-    <t>21/10/2024 20:25:38</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:29:16</t>
-  </si>
-  <si>
-    <t>21/10/2024 20:41:49</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:31:20</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:10:56</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:39:02</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:13:26</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:46:00</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:15:30</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:49:29</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:21:50</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:49:31</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:23:10</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:51:46</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:27:49</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:52:46</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:27:51</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:53:30</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:29:55</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:54:03</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:35:01</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:55:01</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:45:13</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:55:25</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:46:17</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:56:07</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:49:07</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:56:41</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:49:45</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:57:02</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:52:04</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:58:16</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:53:03</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:59:35</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:53:46</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:00:57</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:54:18</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:01:29</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:55:09</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:01:50</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:55:42</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:02:08</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:55:43</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:02:36</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:56:26</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:03:12</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:58:00</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:07:02</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:58:32</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:10:42</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:59:53</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:12:00</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:01:11</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:12:03</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:01:32</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:13:21</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:02:03</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:13:57</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:02:11</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:15:01</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:02:51</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:15:25</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:03:25</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:18:46</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:10:13</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:21:11</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:10:14</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:22:04</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:11:00</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:22:47</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:12:19</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:23:13</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:13:37</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:25:08</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:14:13</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:26:08</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:15:12</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:26:49</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:15:14</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:27:39</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:15:53</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:28:21</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:19:02</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:29:11</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:21:28</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:29:48</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:22:24</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:30:22</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:23:01</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:31:54</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:23:03</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:32:43</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:23:34</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:34:05</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:23:36</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:35:20</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:25:47</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:37:37</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:26:21</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:40:58</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:27:03</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:41:25</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:27:52</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:41:49</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:28:35</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:42:19</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:28:36</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:44:34</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:29:26</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:45:01</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:30:04</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:45:31</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:30:37</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:46:55</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:32:07</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:48:16</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:33:37</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:49:04</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:34:28</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:49:42</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:35:48</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:50:04</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:37:50</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:50:46</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:41:11</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:52:28</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:41:39</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:53:01</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:42:04</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:53:51</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:42:39</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:54:20</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:43:45</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:55:15</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:44:47</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:55:39</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:45:17</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:56:39</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:45:43</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:57:47</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:47:11</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:58:41</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:48:34</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:59:10</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:49:15</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:59:37</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:49:55</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:00:05</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:50:16</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:00:56</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:50:59</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:01:54</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:52:50</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:03:40</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:53:15</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:04:21</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:54:05</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:05:04</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:54:36</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:06:02</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:55:28</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:10:35</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:56:25</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:11:09</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:56:53</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:11:40</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:58:01</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:12:16</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:58:56</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:12:43</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:59:25</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:13:18</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:59:51</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:16:34</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:00:18</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:20:09</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:01:08</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:20:41</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:02:06</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:31:14</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:03:54</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:32:20</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:04:34</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:32:56</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:05:17</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:34:03</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:06:15</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:35:02</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:10:46</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:36:01</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:11:22</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:37:00</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:11:51</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:37:30</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:12:28</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:37:59</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:12:55</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:38:34</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:13:45</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:46:05</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:16:46</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:46:45</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:20:22</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:47:32</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:22:38</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:48:19</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:29:51</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:51:43</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:31:28</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:54:52</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:32:34</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:55:45</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:33:28</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:56:49</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:34:18</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:57:29</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:35:14</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:58:19</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:36:13</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:00:00</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:37:12</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:02:23</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:37:42</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:03:09</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:38:10</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:08:10</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:38:46</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:09:54</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:46:17</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:11:17</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:47:09</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:15:42</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:47:49</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:16:12</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:49:52</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:20:34</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:52:35</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:32:28</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:55:13</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:39:02</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:56:17</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:40:04</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:57:09</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:51:12</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:57:51</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:57:53</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:58:34</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:58:26</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:00:38</t>
-  </si>
-  <si>
-    <t>22/10/2024 01:10:53</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:02:59</t>
-  </si>
-  <si>
-    <t>22/10/2024 01:13:37</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:05:41</t>
-  </si>
-  <si>
-    <t>22/10/2024 01:15:46</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:08:29</t>
-  </si>
-  <si>
-    <t>22/10/2024 01:16:13</t>
-  </si>
-  <si>
     <t>22/10/2024 00:14:21</t>
   </si>
   <si>
+    <t>22/10/2024 01:37:38</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:20:20</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>22/10/2024 00:16:01</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:20:20</t>
-  </si>
-  <si>
     <t>22/10/2024 00:31:52</t>
   </si>
   <si>
@@ -1674,6 +1680,9 @@
   </si>
   <si>
     <t>22/10/2024 01:16:22</t>
+  </si>
+  <si>
+    <t>22/10/2024 01:36:39</t>
   </si>
 </sst>
 </file>
@@ -1721,7 +1730,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D285"/>
+  <dimension ref="A1:D286"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -5509,10 +5518,10 @@
     </row>
     <row r="271">
       <c r="A271" t="s" s="1">
-        <v>236</v>
+        <v>539</v>
       </c>
       <c r="B271" t="s" s="1">
-        <v>237</v>
+        <v>540</v>
       </c>
       <c r="C271" t="s" s="0">
         <v>238</v>
@@ -5523,10 +5532,10 @@
     </row>
     <row r="272">
       <c r="A272" t="s" s="1">
-        <v>539</v>
-      </c>
-      <c r="B272" t="s" s="0">
-        <v>540</v>
+        <v>541</v>
+      </c>
+      <c r="B272" t="s" s="1">
+        <v>542</v>
       </c>
       <c r="C272" t="s" s="0">
         <v>238</v>
@@ -5537,10 +5546,10 @@
     </row>
     <row r="273">
       <c r="A273" t="s" s="1">
-        <v>541</v>
-      </c>
-      <c r="B273" t="s" s="0">
-        <v>540</v>
+        <v>236</v>
+      </c>
+      <c r="B273" t="s" s="1">
+        <v>237</v>
       </c>
       <c r="C273" t="s" s="0">
         <v>238</v>
@@ -5551,10 +5560,10 @@
     </row>
     <row r="274">
       <c r="A274" t="s" s="1">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B274" t="s" s="0">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="C274" t="s" s="0">
         <v>238</v>
@@ -5565,10 +5574,10 @@
     </row>
     <row r="275">
       <c r="A275" t="s" s="1">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="B275" t="s" s="0">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="C275" t="s" s="0">
         <v>238</v>
@@ -5579,10 +5588,10 @@
     </row>
     <row r="276">
       <c r="A276" t="s" s="1">
+        <v>546</v>
+      </c>
+      <c r="B276" t="s" s="0">
         <v>544</v>
-      </c>
-      <c r="B276" t="s" s="0">
-        <v>540</v>
       </c>
       <c r="C276" t="s" s="0">
         <v>238</v>
@@ -5593,10 +5602,10 @@
     </row>
     <row r="277">
       <c r="A277" t="s" s="1">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="B277" t="s" s="0">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="C277" t="s" s="0">
         <v>238</v>
@@ -5607,10 +5616,10 @@
     </row>
     <row r="278">
       <c r="A278" t="s" s="1">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="B278" t="s" s="0">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="C278" t="s" s="0">
         <v>238</v>
@@ -5621,10 +5630,10 @@
     </row>
     <row r="279">
       <c r="A279" t="s" s="1">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="B279" t="s" s="0">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="C279" t="s" s="0">
         <v>238</v>
@@ -5635,10 +5644,10 @@
     </row>
     <row r="280">
       <c r="A280" t="s" s="1">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="B280" t="s" s="0">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="C280" t="s" s="0">
         <v>238</v>
@@ -5649,10 +5658,10 @@
     </row>
     <row r="281">
       <c r="A281" t="s" s="1">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="B281" t="s" s="0">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="C281" t="s" s="0">
         <v>238</v>
@@ -5663,10 +5672,10 @@
     </row>
     <row r="282">
       <c r="A282" t="s" s="1">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="B282" t="s" s="0">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="C282" t="s" s="0">
         <v>238</v>
@@ -5677,10 +5686,10 @@
     </row>
     <row r="283">
       <c r="A283" t="s" s="1">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="B283" t="s" s="0">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="C283" t="s" s="0">
         <v>238</v>
@@ -5691,10 +5700,10 @@
     </row>
     <row r="284">
       <c r="A284" t="s" s="1">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="B284" t="s" s="0">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="C284" t="s" s="0">
         <v>238</v>
@@ -5705,15 +5714,29 @@
     </row>
     <row r="285">
       <c r="A285" t="s" s="1">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="B285" t="s" s="0">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="C285" t="s" s="0">
         <v>238</v>
       </c>
       <c r="D285" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="s" s="1">
+        <v>556</v>
+      </c>
+      <c r="B286" t="s" s="0">
+        <v>544</v>
+      </c>
+      <c r="C286" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="D286" t="s" s="0">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
OPTIMIZACION DE PROCESOS Y DISEÑO NO.9
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/LOGGIN.xlsx
+++ b/ProyectoPooDist/excels/LOGGIN.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="942">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1988" uniqueCount="991">
   <si>
     <t>Tiempo Entrada</t>
   </si>
@@ -722,2122 +722,2269 @@
     <t>20/10/2024 17:42:55</t>
   </si>
   <si>
+    <t>23/10/2024 16:59:12</t>
+  </si>
+  <si>
+    <t>23/10/2024 18:13:23</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>21/10/2024 06:19:20</t>
+  </si>
+  <si>
+    <t>21/10/2024 06:20:32</t>
+  </si>
+  <si>
+    <t>21/10/2024 06:29:18</t>
+  </si>
+  <si>
+    <t>21/10/2024 06:30:52</t>
+  </si>
+  <si>
+    <t>21/10/2024 06:50:12</t>
+  </si>
+  <si>
+    <t>21/10/2024 06:51:02</t>
+  </si>
+  <si>
+    <t>21/10/2024 06:51:46</t>
+  </si>
+  <si>
+    <t>21/10/2024 06:52:35</t>
+  </si>
+  <si>
+    <t>21/10/2024 07:55:32</t>
+  </si>
+  <si>
+    <t>21/10/2024 07:56:34</t>
+  </si>
+  <si>
+    <t>21/10/2024 08:21:11</t>
+  </si>
+  <si>
+    <t>21/10/2024 08:26:04</t>
+  </si>
+  <si>
+    <t>21/10/2024 08:22:37</t>
+  </si>
+  <si>
+    <t>21/10/2024 08:30:58</t>
+  </si>
+  <si>
+    <t>21/10/2024 08:25:17</t>
+  </si>
+  <si>
+    <t>21/10/2024 18:51:53</t>
+  </si>
+  <si>
+    <t>21/10/2024 08:26:24</t>
+  </si>
+  <si>
+    <t>21/10/2024 18:51:54</t>
+  </si>
+  <si>
+    <t>21/10/2024 08:28:36</t>
+  </si>
+  <si>
+    <t>21/10/2024 19:28:58</t>
+  </si>
+  <si>
+    <t>21/10/2024 08:32:33</t>
+  </si>
+  <si>
+    <t>21/10/2024 19:31:36</t>
+  </si>
+  <si>
+    <t>21/10/2024 08:35:11</t>
+  </si>
+  <si>
+    <t>21/10/2024 19:33:13</t>
+  </si>
+  <si>
+    <t>21/10/2024 18:51:42</t>
+  </si>
+  <si>
+    <t>21/10/2024 19:39:01</t>
+  </si>
+  <si>
+    <t>21/10/2024 19:30:29</t>
+  </si>
+  <si>
+    <t>21/10/2024 19:45:27</t>
+  </si>
+  <si>
+    <t>21/10/2024 19:31:56</t>
+  </si>
+  <si>
+    <t>21/10/2024 20:24:36</t>
+  </si>
+  <si>
+    <t>21/10/2024 19:35:20</t>
+  </si>
+  <si>
+    <t>21/10/2024 20:25:20</t>
+  </si>
+  <si>
+    <t>21/10/2024 19:39:13</t>
+  </si>
+  <si>
+    <t>21/10/2024 20:26:27</t>
+  </si>
+  <si>
+    <t>21/10/2024 20:19:17</t>
+  </si>
+  <si>
+    <t>21/10/2024 20:42:29</t>
+  </si>
+  <si>
+    <t>21/10/2024 20:20:27</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:13:00</t>
+  </si>
+  <si>
+    <t>21/10/2024 20:21:24</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:15:05</t>
+  </si>
+  <si>
+    <t>21/10/2024 20:22:31</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:16:31</t>
+  </si>
+  <si>
+    <t>21/10/2024 20:24:52</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:22:27</t>
+  </si>
+  <si>
+    <t>21/10/2024 20:25:38</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:29:16</t>
+  </si>
+  <si>
+    <t>21/10/2024 20:41:49</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:31:20</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:10:56</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:39:02</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:13:26</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:46:00</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:15:30</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:49:29</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:21:50</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:49:31</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:23:10</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:51:46</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:27:49</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:52:46</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:27:51</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:53:30</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:29:55</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:54:03</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:35:01</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:55:01</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:45:13</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:55:25</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:46:17</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:56:07</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:49:07</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:56:41</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:49:45</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:57:02</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:52:04</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:58:16</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:53:03</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:59:35</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:53:46</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:00:57</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:54:18</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:01:29</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:55:09</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:01:50</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:55:42</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:02:08</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:55:43</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:02:36</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:56:26</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:03:12</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:58:00</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:07:02</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:58:32</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:10:42</t>
+  </si>
+  <si>
+    <t>21/10/2024 21:59:53</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:12:00</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:01:11</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:12:03</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:01:32</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:13:21</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:02:03</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:13:57</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:02:11</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:15:01</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:02:51</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:15:25</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:03:25</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:18:46</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:10:13</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:21:11</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:10:14</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:22:04</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:11:00</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:22:47</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:12:19</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:23:13</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:13:37</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:25:08</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:14:13</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:26:08</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:15:12</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:26:49</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:15:14</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:27:39</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:15:53</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:28:21</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:19:02</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:29:11</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:21:28</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:29:48</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:22:24</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:30:22</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:23:01</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:31:54</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:23:03</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:32:43</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:23:34</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:34:05</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:23:36</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:35:20</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:25:47</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:37:37</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:26:21</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:40:58</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:27:03</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:41:25</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:27:52</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:41:49</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:28:35</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:42:19</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:28:36</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:44:34</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:29:26</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:45:01</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:30:04</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:45:31</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:30:37</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:46:55</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:32:07</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:48:16</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:33:37</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:49:04</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:34:28</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:49:42</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:35:48</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:50:04</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:37:50</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:50:46</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:41:11</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:52:28</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:41:39</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:53:01</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:42:04</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:53:51</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:42:39</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:54:20</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:43:45</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:55:15</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:44:47</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:55:39</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:45:17</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:56:39</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:45:43</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:57:47</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:47:11</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:58:41</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:48:34</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:59:10</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:49:15</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:59:37</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:49:55</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:00:05</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:50:16</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:00:56</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:50:59</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:01:54</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:52:50</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:03:40</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:53:15</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:04:21</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:54:05</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:05:04</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:54:36</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:06:02</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:55:28</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:10:35</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:56:25</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:11:09</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:56:53</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:11:40</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:58:01</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:12:16</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:58:56</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:12:43</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:59:25</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:13:18</t>
+  </si>
+  <si>
+    <t>21/10/2024 22:59:51</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:16:34</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:00:18</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:20:09</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:01:08</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:20:41</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:02:06</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:31:14</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:03:54</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:32:20</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:04:34</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:32:56</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:05:17</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:34:03</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:06:15</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:35:02</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:10:46</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:36:01</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:11:22</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:37:00</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:11:51</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:37:30</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:12:28</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:37:59</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:12:55</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:38:34</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:13:45</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:46:05</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:16:46</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:46:45</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:20:22</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:47:32</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:22:38</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:48:19</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:29:51</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:51:43</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:31:28</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:54:52</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:32:34</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:55:45</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:33:28</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:56:49</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:34:18</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:57:29</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:35:14</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:58:19</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:36:13</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:00:00</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:37:12</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:02:23</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:37:42</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:03:09</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:38:10</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:08:10</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:38:46</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:09:54</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:46:17</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:11:17</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:47:09</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:15:42</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:47:49</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:16:12</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:49:52</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:20:34</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:52:35</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:32:28</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:55:13</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:39:02</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:56:17</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:40:04</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:57:09</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:51:12</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:57:51</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:57:53</t>
+  </si>
+  <si>
+    <t>21/10/2024 23:58:34</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:58:26</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:00:38</t>
+  </si>
+  <si>
+    <t>22/10/2024 01:10:53</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:02:59</t>
+  </si>
+  <si>
+    <t>22/10/2024 01:13:37</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:05:41</t>
+  </si>
+  <si>
+    <t>22/10/2024 01:15:46</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:08:29</t>
+  </si>
+  <si>
+    <t>22/10/2024 01:16:13</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:11:00</t>
+  </si>
+  <si>
+    <t>22/10/2024 01:16:32</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:14:21</t>
+  </si>
+  <si>
+    <t>22/10/2024 01:37:38</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:16:01</t>
+  </si>
+  <si>
+    <t>22/10/2024 01:39:19</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:20:20</t>
+  </si>
+  <si>
+    <t>22/10/2024 06:29:19</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:31:52</t>
+  </si>
+  <si>
+    <t>22/10/2024 06:36:55</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:38:52</t>
+  </si>
+  <si>
+    <t>22/10/2024 06:42:28</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:39:35</t>
+  </si>
+  <si>
+    <t>22/10/2024 06:46:49</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:50:31</t>
+  </si>
+  <si>
+    <t>22/10/2024 06:48:02</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:55:02</t>
+  </si>
+  <si>
+    <t>22/10/2024 06:50:40</t>
+  </si>
+  <si>
+    <t>22/10/2024 00:58:08</t>
+  </si>
+  <si>
+    <t>22/10/2024 06:51:11</t>
+  </si>
+  <si>
+    <t>22/10/2024 01:10:37</t>
+  </si>
+  <si>
+    <t>22/10/2024 06:56:42</t>
+  </si>
+  <si>
+    <t>22/10/2024 01:13:21</t>
+  </si>
+  <si>
+    <t>22/10/2024 07:00:20</t>
+  </si>
+  <si>
+    <t>22/10/2024 01:13:50</t>
+  </si>
+  <si>
+    <t>22/10/2024 07:04:08</t>
+  </si>
+  <si>
+    <t>22/10/2024 01:16:00</t>
+  </si>
+  <si>
+    <t>22/10/2024 09:57:51</t>
+  </si>
+  <si>
+    <t>22/10/2024 01:16:22</t>
+  </si>
+  <si>
+    <t>22/10/2024 09:59:21</t>
+  </si>
+  <si>
+    <t>22/10/2024 01:36:39</t>
+  </si>
+  <si>
+    <t>22/10/2024 10:00:56</t>
+  </si>
+  <si>
+    <t>22/10/2024 06:22:35</t>
+  </si>
+  <si>
+    <t>22/10/2024 10:01:43</t>
+  </si>
+  <si>
+    <t>22/10/2024 06:38:06</t>
+  </si>
+  <si>
+    <t>22/10/2024 10:06:01</t>
+  </si>
+  <si>
+    <t>22/10/2024 06:45:55</t>
+  </si>
+  <si>
+    <t>22/10/2024 10:06:36</t>
+  </si>
+  <si>
+    <t>22/10/2024 06:47:30</t>
+  </si>
+  <si>
+    <t>22/10/2024 10:07:13</t>
+  </si>
+  <si>
+    <t>22/10/2024 06:48:30</t>
+  </si>
+  <si>
+    <t>22/10/2024 10:12:23</t>
+  </si>
+  <si>
+    <t>22/10/2024 06:51:00</t>
+  </si>
+  <si>
+    <t>22/10/2024 10:18:52</t>
+  </si>
+  <si>
+    <t>22/10/2024 06:56:38</t>
+  </si>
+  <si>
+    <t>22/10/2024 10:19:40</t>
+  </si>
+  <si>
+    <t>22/10/2024 06:59:55</t>
+  </si>
+  <si>
+    <t>22/10/2024 10:20:18</t>
+  </si>
+  <si>
+    <t>22/10/2024 07:01:21</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:04:33</t>
+  </si>
+  <si>
+    <t>22/10/2024 09:53:59</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:05:33</t>
+  </si>
+  <si>
+    <t>22/10/2024 09:58:13</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:06:38</t>
+  </si>
+  <si>
+    <t>22/10/2024 10:00:03</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:07:12</t>
+  </si>
+  <si>
+    <t>22/10/2024 10:01:11</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:07:53</t>
+  </si>
+  <si>
+    <t>22/10/2024 10:03:34</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:08:40</t>
+  </si>
+  <si>
+    <t>22/10/2024 10:06:15</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:09:13</t>
+  </si>
+  <si>
+    <t>22/10/2024 10:06:54</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:10:50</t>
+  </si>
+  <si>
+    <t>22/10/2024 10:12:10</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:11:19</t>
+  </si>
+  <si>
+    <t>22/10/2024 10:18:30</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:11:58</t>
+  </si>
+  <si>
+    <t>22/10/2024 10:19:05</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:14:13</t>
+  </si>
+  <si>
+    <t>22/10/2024 10:19:52</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:14:16</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:04:05</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:14:54</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:04:48</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:16:20</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:06:10</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:16:51</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:06:53</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:17:21</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:07:31</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:17:54</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:08:14</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:18:20</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:08:59</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:18:45</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:09:35</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:19:09</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:11:04</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:20:16</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:11:36</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:20:55</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:12:13</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:21:27</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:12:15</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:22:13</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:13:30</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:22:44</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:14:30</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:23:08</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:15:08</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:23:50</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:16:37</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:24:17</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:17:05</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:24:55</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:17:34</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:25:23</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:18:07</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:27:05</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:18:31</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:27:38</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:18:57</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:28:26</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:19:21</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:28:51</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:20:31</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:29:18</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:21:12</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:29:42</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:21:40</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:30:07</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:22:26</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:30:26</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:22:57</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:40:23</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:23:20</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:42:28</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:24:03</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:55:35</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:24:29</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:04:43</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:25:08</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:25:34</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:25:36</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:30:13</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:27:20</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:34:51</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:27:52</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:35:53</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:28:39</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:38:07</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:29:05</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:41:29</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:29:32</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:44:01</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:29:56</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:45:17</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:30:20</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:52:01</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:40:18</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:54:06</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:40:25</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:57:58</t>
+  </si>
+  <si>
+    <t>22/10/2024 11:56:37</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:59:29</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:24:54</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:03:04</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:25:17</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:04:29</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:25:50</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:13:00</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:28:17</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:15:38</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:35:11</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:16:27</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:37:45</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:16:57</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:39:01</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:19:30</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:41:52</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:24:35</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:44:19</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:25:54</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:45:48</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:30:58</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:53:00</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:31:38</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:53:02</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:32:37</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:54:31</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:43:12</t>
+  </si>
+  <si>
+    <t>22/10/2024 12:58:07</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:48:58</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:00:33</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:50:20</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:00:35</t>
+  </si>
+  <si>
+    <t>22/10/2024 14:15:07</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:03:15</t>
+  </si>
+  <si>
+    <t>22/10/2024 15:42:38</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:11:34</t>
+  </si>
+  <si>
+    <t>22/10/2024 15:46:08</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:14:32</t>
+  </si>
+  <si>
+    <t>22/10/2024 15:46:10</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:16:15</t>
+  </si>
+  <si>
+    <t>22/10/2024 15:47:54</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:17:05</t>
+  </si>
+  <si>
+    <t>22/10/2024 15:57:39</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:22:11</t>
+  </si>
+  <si>
+    <t>22/10/2024 15:59:37</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:24:44</t>
+  </si>
+  <si>
+    <t>22/10/2024 16:06:21</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:24:46</t>
+  </si>
+  <si>
+    <t>22/10/2024 16:09:58</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:27:01</t>
+  </si>
+  <si>
+    <t>22/10/2024 16:12:18</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:31:10</t>
+  </si>
+  <si>
+    <t>22/10/2024 16:20:31</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:32:24</t>
+  </si>
+  <si>
+    <t>22/10/2024 16:29:39</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:42:19</t>
+  </si>
+  <si>
+    <t>22/10/2024 16:39:43</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:43:33</t>
+  </si>
+  <si>
+    <t>22/10/2024 16:39:51</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:49:27</t>
+  </si>
+  <si>
+    <t>22/10/2024 16:41:50</t>
+  </si>
+  <si>
+    <t>22/10/2024 13:51:06</t>
+  </si>
+  <si>
+    <t>22/10/2024 16:43:42</t>
+  </si>
+  <si>
+    <t>22/10/2024 15:40:38</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:02:27</t>
+  </si>
+  <si>
+    <t>22/10/2024 15:44:03</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:20:35</t>
+  </si>
+  <si>
+    <t>22/10/2024 15:47:00</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:25:38</t>
+  </si>
+  <si>
+    <t>22/10/2024 15:48:08</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:26:12</t>
+  </si>
+  <si>
+    <t>22/10/2024 15:58:55</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:27:05</t>
+  </si>
+  <si>
+    <t>22/10/2024 16:04:56</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:27:50</t>
+  </si>
+  <si>
+    <t>22/10/2024 16:08:06</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:28:30</t>
+  </si>
+  <si>
+    <t>22/10/2024 16:10:40</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:31:45</t>
+  </si>
+  <si>
+    <t>22/10/2024 16:14:52</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:32:33</t>
+  </si>
+  <si>
+    <t>22/10/2024 16:23:33</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:32:34</t>
+  </si>
+  <si>
+    <t>22/10/2024 16:35:02</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:38:59</t>
+  </si>
+  <si>
+    <t>22/10/2024 16:36:16</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:42:50</t>
+  </si>
+  <si>
+    <t>22/10/2024 16:38:30</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:45:32</t>
+  </si>
+  <si>
+    <t>22/10/2024 16:40:08</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:46:02</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:01:41</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:46:04</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:17:50</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:08:39</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:20:59</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:11:17</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:26:03</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:13:49</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:27:21</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:15:40</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:28:21</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:17:46</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:31:01</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:20:23</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:32:14</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:29:33</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:38:35</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:29:38</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:42:14</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:29:56</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:43:23</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:34:24</t>
+  </si>
+  <si>
+    <t>22/10/2024 17:45:45</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:43:10</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:08:19</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:57:51</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:10:26</t>
+  </si>
+  <si>
+    <t>22/10/2024 19:12:05</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:10:52</t>
+  </si>
+  <si>
+    <t>22/10/2024 19:17:28</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:13:37</t>
+  </si>
+  <si>
+    <t>22/10/2024 19:19:41</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:17:33</t>
+  </si>
+  <si>
+    <t>22/10/2024 19:20:24</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:18:54</t>
+  </si>
+  <si>
+    <t>22/10/2024 19:24:01</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:20:39</t>
+  </si>
+  <si>
+    <t>23/10/2024 06:36:28</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:29:15</t>
+  </si>
+  <si>
+    <t>23/10/2024 06:39:48</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:29:47</t>
+  </si>
+  <si>
+    <t>23/10/2024 06:42:05</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:30:33</t>
+  </si>
+  <si>
+    <t>23/10/2024 06:43:07</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:38:32</t>
+  </si>
+  <si>
+    <t>23/10/2024 06:44:55</t>
+  </si>
+  <si>
+    <t>22/10/2024 18:54:24</t>
+  </si>
+  <si>
+    <t>23/10/2024 06:46:28</t>
+  </si>
+  <si>
+    <t>22/10/2024 19:08:58</t>
+  </si>
+  <si>
+    <t>23/10/2024 06:57:31</t>
+  </si>
+  <si>
+    <t>22/10/2024 19:16:56</t>
+  </si>
+  <si>
+    <t>23/10/2024 07:01:14</t>
+  </si>
+  <si>
+    <t>22/10/2024 19:20:00</t>
+  </si>
+  <si>
+    <t>23/10/2024 07:08:33</t>
+  </si>
+  <si>
+    <t>22/10/2024 19:21:54</t>
+  </si>
+  <si>
+    <t>23/10/2024 07:48:04</t>
+  </si>
+  <si>
+    <t>23/10/2024 06:32:12</t>
+  </si>
+  <si>
+    <t>23/10/2024 07:49:24</t>
+  </si>
+  <si>
+    <t>23/10/2024 06:39:27</t>
+  </si>
+  <si>
+    <t>23/10/2024 07:55:13</t>
+  </si>
+  <si>
+    <t>23/10/2024 06:41:10</t>
+  </si>
+  <si>
+    <t>23/10/2024 07:55:43</t>
+  </si>
+  <si>
+    <t>23/10/2024 06:42:57</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:04:56</t>
+  </si>
+  <si>
+    <t>23/10/2024 06:44:31</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:34:25</t>
+  </si>
+  <si>
+    <t>23/10/2024 06:45:26</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:36:04</t>
+  </si>
+  <si>
+    <t>23/10/2024 06:57:23</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:36:08</t>
+  </si>
+  <si>
+    <t>23/10/2024 06:57:44</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:36:57</t>
+  </si>
+  <si>
+    <t>23/10/2024 07:03:39</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:37:45</t>
+  </si>
+  <si>
+    <t>23/10/2024 07:03:40</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:38:25</t>
+  </si>
+  <si>
+    <t>23/10/2024 07:47:41</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:39:03</t>
+  </si>
+  <si>
+    <t>23/10/2024 07:49:07</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:39:48</t>
+  </si>
+  <si>
+    <t>23/10/2024 07:49:39</t>
+  </si>
+  <si>
+    <t>23/10/2024 07:49:48</t>
+  </si>
+  <si>
+    <t>pedro.lopez&amp;pineed</t>
+  </si>
+  <si>
+    <t>PILOTO</t>
+  </si>
+  <si>
+    <t>23/10/2024 07:55:08</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:44:48</t>
+  </si>
+  <si>
+    <t>23/10/2024 07:55:28</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:46:17</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:13:06</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:13:53</t>
+  </si>
+  <si>
+    <t>ana.martinez&amp;pineed</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:01:45</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:46:39</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:33:03</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:47:38</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:34:28</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:48:29</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:35:03</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:49:58</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:36:34</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:50:59</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:37:21</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:56:06</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:38:10</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:07:12</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:38:50</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:08:23</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:39:26</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:18:04</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:40:27</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:18:08</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:45:33</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:21:31</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:47:13</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:23:01</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:48:05</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:56:28</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:49:18</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:56:30</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:50:23</t>
+  </si>
+  <si>
+    <t>23/10/2024 10:06:58</t>
+  </si>
+  <si>
+    <t>23/10/2024 08:51:22</t>
+  </si>
+  <si>
+    <t>23/10/2024 10:16:03</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:06:57</t>
+  </si>
+  <si>
+    <t>23/10/2024 10:24:12</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:07:29</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:07:44</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:07:46</t>
+  </si>
+  <si>
+    <t>23/10/2024 10:25:11</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:08:42</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:09:35</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:10:23</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:12:20</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:13:58</t>
+  </si>
+  <si>
+    <t>23/10/2024 10:27:26</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:20:54</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:21:07</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>SECRETARIA</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:21:09</t>
+  </si>
+  <si>
+    <t>23/10/2024 10:46:02</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:34:22</t>
+  </si>
+  <si>
+    <t>23/10/2024 10:57:34</t>
+  </si>
+  <si>
+    <t>23/10/2024 09:50:36</t>
+  </si>
+  <si>
+    <t>23/10/2024 11:02:22</t>
+  </si>
+  <si>
+    <t>23/10/2024 10:13:51</t>
+  </si>
+  <si>
+    <t>23/10/2024 11:12:59</t>
+  </si>
+  <si>
+    <t>23/10/2024 10:23:06</t>
+  </si>
+  <si>
+    <t>23/10/2024 11:17:18</t>
+  </si>
+  <si>
     <t>23/10/2024 10:24:47</t>
   </si>
   <si>
     <t>23/10/2024 11:21:40</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>21/10/2024 06:19:20</t>
-  </si>
-  <si>
-    <t>21/10/2024 06:20:32</t>
-  </si>
-  <si>
-    <t>21/10/2024 06:29:18</t>
-  </si>
-  <si>
-    <t>21/10/2024 06:30:52</t>
-  </si>
-  <si>
-    <t>21/10/2024 06:50:12</t>
-  </si>
-  <si>
-    <t>21/10/2024 06:51:02</t>
-  </si>
-  <si>
-    <t>21/10/2024 06:51:46</t>
-  </si>
-  <si>
-    <t>21/10/2024 06:52:35</t>
-  </si>
-  <si>
-    <t>21/10/2024 07:55:32</t>
-  </si>
-  <si>
-    <t>21/10/2024 07:56:34</t>
-  </si>
-  <si>
-    <t>21/10/2024 08:21:11</t>
-  </si>
-  <si>
-    <t>21/10/2024 08:26:04</t>
-  </si>
-  <si>
-    <t>21/10/2024 08:22:37</t>
-  </si>
-  <si>
-    <t>21/10/2024 08:30:58</t>
-  </si>
-  <si>
-    <t>21/10/2024 08:25:17</t>
-  </si>
-  <si>
-    <t>21/10/2024 18:51:53</t>
-  </si>
-  <si>
-    <t>21/10/2024 08:26:24</t>
-  </si>
-  <si>
-    <t>21/10/2024 18:51:54</t>
-  </si>
-  <si>
-    <t>21/10/2024 08:28:36</t>
-  </si>
-  <si>
-    <t>21/10/2024 19:28:58</t>
-  </si>
-  <si>
-    <t>21/10/2024 08:32:33</t>
-  </si>
-  <si>
-    <t>21/10/2024 19:31:36</t>
-  </si>
-  <si>
-    <t>21/10/2024 08:35:11</t>
-  </si>
-  <si>
-    <t>21/10/2024 19:33:13</t>
-  </si>
-  <si>
-    <t>21/10/2024 18:51:42</t>
-  </si>
-  <si>
-    <t>21/10/2024 19:39:01</t>
-  </si>
-  <si>
-    <t>21/10/2024 19:30:29</t>
-  </si>
-  <si>
-    <t>21/10/2024 19:45:27</t>
-  </si>
-  <si>
-    <t>21/10/2024 19:31:56</t>
-  </si>
-  <si>
-    <t>21/10/2024 20:24:36</t>
-  </si>
-  <si>
-    <t>21/10/2024 19:35:20</t>
-  </si>
-  <si>
-    <t>21/10/2024 20:25:20</t>
-  </si>
-  <si>
-    <t>21/10/2024 19:39:13</t>
-  </si>
-  <si>
-    <t>21/10/2024 20:26:27</t>
-  </si>
-  <si>
-    <t>21/10/2024 20:19:17</t>
-  </si>
-  <si>
-    <t>21/10/2024 20:42:29</t>
-  </si>
-  <si>
-    <t>21/10/2024 20:20:27</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:13:00</t>
-  </si>
-  <si>
-    <t>21/10/2024 20:21:24</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:15:05</t>
-  </si>
-  <si>
-    <t>21/10/2024 20:22:31</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:16:31</t>
-  </si>
-  <si>
-    <t>21/10/2024 20:24:52</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:22:27</t>
-  </si>
-  <si>
-    <t>21/10/2024 20:25:38</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:29:16</t>
-  </si>
-  <si>
-    <t>21/10/2024 20:41:49</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:31:20</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:10:56</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:39:02</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:13:26</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:46:00</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:15:30</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:49:29</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:21:50</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:49:31</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:23:10</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:51:46</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:27:49</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:52:46</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:27:51</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:53:30</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:29:55</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:54:03</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:35:01</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:55:01</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:45:13</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:55:25</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:46:17</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:56:07</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:49:07</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:56:41</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:49:45</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:57:02</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:52:04</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:58:16</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:53:03</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:59:35</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:53:46</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:00:57</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:54:18</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:01:29</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:55:09</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:01:50</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:55:42</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:02:08</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:55:43</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:02:36</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:56:26</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:03:12</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:58:00</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:07:02</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:58:32</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:10:42</t>
-  </si>
-  <si>
-    <t>21/10/2024 21:59:53</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:12:00</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:01:11</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:12:03</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:01:32</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:13:21</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:02:03</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:13:57</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:02:11</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:15:01</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:02:51</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:15:25</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:03:25</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:18:46</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:10:13</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:21:11</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:10:14</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:22:04</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:11:00</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:22:47</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:12:19</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:23:13</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:13:37</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:25:08</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:14:13</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:26:08</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:15:12</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:26:49</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:15:14</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:27:39</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:15:53</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:28:21</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:19:02</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:29:11</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:21:28</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:29:48</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:22:24</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:30:22</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:23:01</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:31:54</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:23:03</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:32:43</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:23:34</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:34:05</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:23:36</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:35:20</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:25:47</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:37:37</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:26:21</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:40:58</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:27:03</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:41:25</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:27:52</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:41:49</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:28:35</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:42:19</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:28:36</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:44:34</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:29:26</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:45:01</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:30:04</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:45:31</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:30:37</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:46:55</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:32:07</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:48:16</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:33:37</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:49:04</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:34:28</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:49:42</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:35:48</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:50:04</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:37:50</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:50:46</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:41:11</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:52:28</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:41:39</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:53:01</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:42:04</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:53:51</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:42:39</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:54:20</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:43:45</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:55:15</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:44:47</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:55:39</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:45:17</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:56:39</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:45:43</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:57:47</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:47:11</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:58:41</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:48:34</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:59:10</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:49:15</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:59:37</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:49:55</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:00:05</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:50:16</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:00:56</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:50:59</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:01:54</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:52:50</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:03:40</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:53:15</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:04:21</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:54:05</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:05:04</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:54:36</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:06:02</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:55:28</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:10:35</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:56:25</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:11:09</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:56:53</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:11:40</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:58:01</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:12:16</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:58:56</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:12:43</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:59:25</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:13:18</t>
-  </si>
-  <si>
-    <t>21/10/2024 22:59:51</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:16:34</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:00:18</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:20:09</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:01:08</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:20:41</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:02:06</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:31:14</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:03:54</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:32:20</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:04:34</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:32:56</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:05:17</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:34:03</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:06:15</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:35:02</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:10:46</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:36:01</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:11:22</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:37:00</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:11:51</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:37:30</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:12:28</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:37:59</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:12:55</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:38:34</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:13:45</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:46:05</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:16:46</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:46:45</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:20:22</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:47:32</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:22:38</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:48:19</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:29:51</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:51:43</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:31:28</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:54:52</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:32:34</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:55:45</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:33:28</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:56:49</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:34:18</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:57:29</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:35:14</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:58:19</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:36:13</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:00:00</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:37:12</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:02:23</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:37:42</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:03:09</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:38:10</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:08:10</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:38:46</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:09:54</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:46:17</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:11:17</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:47:09</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:15:42</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:47:49</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:16:12</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:49:52</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:20:34</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:52:35</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:32:28</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:55:13</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:39:02</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:56:17</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:40:04</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:57:09</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:51:12</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:57:51</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:57:53</t>
-  </si>
-  <si>
-    <t>21/10/2024 23:58:34</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:58:26</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:00:38</t>
-  </si>
-  <si>
-    <t>22/10/2024 01:10:53</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:02:59</t>
-  </si>
-  <si>
-    <t>22/10/2024 01:13:37</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:05:41</t>
-  </si>
-  <si>
-    <t>22/10/2024 01:15:46</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:08:29</t>
-  </si>
-  <si>
-    <t>22/10/2024 01:16:13</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:11:00</t>
-  </si>
-  <si>
-    <t>22/10/2024 01:16:32</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:14:21</t>
-  </si>
-  <si>
-    <t>22/10/2024 01:37:38</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:16:01</t>
-  </si>
-  <si>
-    <t>22/10/2024 01:39:19</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:20:20</t>
-  </si>
-  <si>
-    <t>22/10/2024 06:29:19</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:31:52</t>
-  </si>
-  <si>
-    <t>22/10/2024 06:36:55</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:38:52</t>
-  </si>
-  <si>
-    <t>22/10/2024 06:42:28</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:39:35</t>
-  </si>
-  <si>
-    <t>22/10/2024 06:46:49</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:50:31</t>
-  </si>
-  <si>
-    <t>22/10/2024 06:48:02</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:55:02</t>
-  </si>
-  <si>
-    <t>22/10/2024 06:50:40</t>
-  </si>
-  <si>
-    <t>22/10/2024 00:58:08</t>
-  </si>
-  <si>
-    <t>22/10/2024 06:51:11</t>
-  </si>
-  <si>
-    <t>22/10/2024 01:10:37</t>
-  </si>
-  <si>
-    <t>22/10/2024 06:56:42</t>
-  </si>
-  <si>
-    <t>22/10/2024 01:13:21</t>
-  </si>
-  <si>
-    <t>22/10/2024 07:00:20</t>
-  </si>
-  <si>
-    <t>22/10/2024 01:13:50</t>
-  </si>
-  <si>
-    <t>22/10/2024 07:04:08</t>
-  </si>
-  <si>
-    <t>22/10/2024 01:16:00</t>
-  </si>
-  <si>
-    <t>22/10/2024 09:57:51</t>
-  </si>
-  <si>
-    <t>22/10/2024 01:16:22</t>
-  </si>
-  <si>
-    <t>22/10/2024 09:59:21</t>
-  </si>
-  <si>
-    <t>22/10/2024 01:36:39</t>
-  </si>
-  <si>
-    <t>22/10/2024 10:00:56</t>
-  </si>
-  <si>
-    <t>22/10/2024 06:22:35</t>
-  </si>
-  <si>
-    <t>22/10/2024 10:01:43</t>
-  </si>
-  <si>
-    <t>22/10/2024 06:38:06</t>
-  </si>
-  <si>
-    <t>22/10/2024 10:06:01</t>
-  </si>
-  <si>
-    <t>22/10/2024 06:45:55</t>
-  </si>
-  <si>
-    <t>22/10/2024 10:06:36</t>
-  </si>
-  <si>
-    <t>22/10/2024 06:47:30</t>
-  </si>
-  <si>
-    <t>22/10/2024 10:07:13</t>
-  </si>
-  <si>
-    <t>22/10/2024 06:48:30</t>
-  </si>
-  <si>
-    <t>22/10/2024 10:12:23</t>
-  </si>
-  <si>
-    <t>22/10/2024 06:51:00</t>
-  </si>
-  <si>
-    <t>22/10/2024 10:18:52</t>
-  </si>
-  <si>
-    <t>22/10/2024 06:56:38</t>
-  </si>
-  <si>
-    <t>22/10/2024 10:19:40</t>
-  </si>
-  <si>
-    <t>22/10/2024 06:59:55</t>
-  </si>
-  <si>
-    <t>22/10/2024 10:20:18</t>
-  </si>
-  <si>
-    <t>22/10/2024 07:01:21</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:04:33</t>
-  </si>
-  <si>
-    <t>22/10/2024 09:53:59</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:05:33</t>
-  </si>
-  <si>
-    <t>22/10/2024 09:58:13</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:06:38</t>
-  </si>
-  <si>
-    <t>22/10/2024 10:00:03</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:07:12</t>
-  </si>
-  <si>
-    <t>22/10/2024 10:01:11</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:07:53</t>
-  </si>
-  <si>
-    <t>22/10/2024 10:03:34</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:08:40</t>
-  </si>
-  <si>
-    <t>22/10/2024 10:06:15</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:09:13</t>
-  </si>
-  <si>
-    <t>22/10/2024 10:06:54</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:10:50</t>
-  </si>
-  <si>
-    <t>22/10/2024 10:12:10</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:11:19</t>
-  </si>
-  <si>
-    <t>22/10/2024 10:18:30</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:11:58</t>
-  </si>
-  <si>
-    <t>22/10/2024 10:19:05</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:14:13</t>
-  </si>
-  <si>
-    <t>22/10/2024 10:19:52</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:14:16</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:04:05</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:14:54</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:04:48</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:16:20</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:06:10</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:16:51</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:06:53</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:17:21</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:07:31</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:17:54</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:08:14</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:18:20</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:08:59</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:18:45</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:09:35</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:19:09</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:11:04</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:20:16</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:11:36</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:20:55</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:12:13</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:21:27</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:12:15</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:22:13</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:13:30</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:22:44</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:14:30</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:23:08</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:15:08</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:23:50</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:16:37</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:24:17</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:17:05</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:24:55</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:17:34</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:25:23</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:18:07</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:27:05</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:18:31</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:27:38</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:18:57</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:28:26</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:19:21</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:28:51</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:20:31</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:29:18</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:21:12</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:29:42</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:21:40</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:30:07</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:22:26</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:30:26</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:22:57</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:40:23</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:23:20</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:42:28</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:24:03</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:55:35</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:24:29</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:04:43</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:25:08</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:25:34</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:25:36</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:30:13</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:27:20</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:34:51</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:27:52</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:35:53</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:28:39</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:38:07</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:29:05</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:41:29</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:29:32</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:44:01</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:29:56</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:45:17</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:30:20</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:52:01</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:40:18</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:54:06</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:40:25</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:57:58</t>
-  </si>
-  <si>
-    <t>22/10/2024 11:56:37</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:59:29</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:24:54</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:03:04</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:25:17</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:04:29</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:25:50</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:13:00</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:28:17</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:15:38</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:35:11</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:16:27</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:37:45</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:16:57</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:39:01</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:19:30</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:41:52</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:24:35</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:44:19</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:25:54</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:45:48</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:30:58</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:53:00</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:31:38</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:53:02</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:32:37</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:54:31</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:43:12</t>
-  </si>
-  <si>
-    <t>22/10/2024 12:58:07</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:48:58</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:00:33</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:50:20</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:00:35</t>
-  </si>
-  <si>
-    <t>22/10/2024 14:15:07</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:03:15</t>
-  </si>
-  <si>
-    <t>22/10/2024 15:42:38</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:11:34</t>
-  </si>
-  <si>
-    <t>22/10/2024 15:46:08</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:14:32</t>
-  </si>
-  <si>
-    <t>22/10/2024 15:46:10</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:16:15</t>
-  </si>
-  <si>
-    <t>22/10/2024 15:47:54</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:17:05</t>
-  </si>
-  <si>
-    <t>22/10/2024 15:57:39</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:22:11</t>
-  </si>
-  <si>
-    <t>22/10/2024 15:59:37</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:24:44</t>
-  </si>
-  <si>
-    <t>22/10/2024 16:06:21</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:24:46</t>
-  </si>
-  <si>
-    <t>22/10/2024 16:09:58</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:27:01</t>
-  </si>
-  <si>
-    <t>22/10/2024 16:12:18</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:31:10</t>
-  </si>
-  <si>
-    <t>22/10/2024 16:20:31</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:32:24</t>
-  </si>
-  <si>
-    <t>22/10/2024 16:29:39</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:42:19</t>
-  </si>
-  <si>
-    <t>22/10/2024 16:39:43</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:43:33</t>
-  </si>
-  <si>
-    <t>22/10/2024 16:39:51</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:49:27</t>
-  </si>
-  <si>
-    <t>22/10/2024 16:41:50</t>
-  </si>
-  <si>
-    <t>22/10/2024 13:51:06</t>
-  </si>
-  <si>
-    <t>22/10/2024 16:43:42</t>
-  </si>
-  <si>
-    <t>22/10/2024 15:40:38</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:02:27</t>
-  </si>
-  <si>
-    <t>22/10/2024 15:44:03</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:20:35</t>
-  </si>
-  <si>
-    <t>22/10/2024 15:47:00</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:25:38</t>
-  </si>
-  <si>
-    <t>22/10/2024 15:48:08</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:26:12</t>
-  </si>
-  <si>
-    <t>22/10/2024 15:58:55</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:27:05</t>
-  </si>
-  <si>
-    <t>22/10/2024 16:04:56</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:27:50</t>
-  </si>
-  <si>
-    <t>22/10/2024 16:08:06</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:28:30</t>
-  </si>
-  <si>
-    <t>22/10/2024 16:10:40</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:31:45</t>
-  </si>
-  <si>
-    <t>22/10/2024 16:14:52</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:32:33</t>
-  </si>
-  <si>
-    <t>22/10/2024 16:23:33</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:32:34</t>
-  </si>
-  <si>
-    <t>22/10/2024 16:35:02</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:38:59</t>
-  </si>
-  <si>
-    <t>22/10/2024 16:36:16</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:42:50</t>
-  </si>
-  <si>
-    <t>22/10/2024 16:38:30</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:45:32</t>
-  </si>
-  <si>
-    <t>22/10/2024 16:40:08</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:46:02</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:01:41</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:46:04</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:17:50</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:08:39</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:20:59</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:11:17</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:26:03</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:13:49</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:27:21</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:15:40</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:28:21</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:17:46</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:31:01</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:20:23</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:32:14</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:29:33</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:38:35</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:29:38</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:42:14</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:29:56</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:43:23</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:34:24</t>
-  </si>
-  <si>
-    <t>22/10/2024 17:45:45</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:43:10</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:08:19</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:57:51</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:10:26</t>
-  </si>
-  <si>
-    <t>22/10/2024 19:12:05</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:10:52</t>
-  </si>
-  <si>
-    <t>22/10/2024 19:17:28</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:13:37</t>
-  </si>
-  <si>
-    <t>22/10/2024 19:19:41</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:17:33</t>
-  </si>
-  <si>
-    <t>22/10/2024 19:20:24</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:18:54</t>
-  </si>
-  <si>
-    <t>22/10/2024 19:24:01</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:20:39</t>
-  </si>
-  <si>
-    <t>23/10/2024 06:36:28</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:29:15</t>
-  </si>
-  <si>
-    <t>23/10/2024 06:39:48</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:29:47</t>
-  </si>
-  <si>
-    <t>23/10/2024 06:42:05</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:30:33</t>
-  </si>
-  <si>
-    <t>23/10/2024 06:43:07</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:38:32</t>
-  </si>
-  <si>
-    <t>23/10/2024 06:44:55</t>
-  </si>
-  <si>
-    <t>22/10/2024 18:54:24</t>
-  </si>
-  <si>
-    <t>23/10/2024 06:46:28</t>
-  </si>
-  <si>
-    <t>22/10/2024 19:08:58</t>
-  </si>
-  <si>
-    <t>23/10/2024 06:57:31</t>
-  </si>
-  <si>
-    <t>22/10/2024 19:16:56</t>
-  </si>
-  <si>
-    <t>23/10/2024 07:01:14</t>
-  </si>
-  <si>
-    <t>22/10/2024 19:20:00</t>
-  </si>
-  <si>
-    <t>23/10/2024 07:08:33</t>
-  </si>
-  <si>
-    <t>22/10/2024 19:21:54</t>
-  </si>
-  <si>
-    <t>23/10/2024 07:48:04</t>
-  </si>
-  <si>
-    <t>23/10/2024 06:32:12</t>
-  </si>
-  <si>
-    <t>23/10/2024 07:49:24</t>
-  </si>
-  <si>
-    <t>23/10/2024 06:39:27</t>
-  </si>
-  <si>
-    <t>23/10/2024 07:55:13</t>
-  </si>
-  <si>
-    <t>23/10/2024 06:41:10</t>
-  </si>
-  <si>
-    <t>23/10/2024 07:55:43</t>
-  </si>
-  <si>
-    <t>23/10/2024 06:42:57</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:04:56</t>
-  </si>
-  <si>
-    <t>23/10/2024 06:44:31</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:34:25</t>
-  </si>
-  <si>
-    <t>23/10/2024 06:45:26</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:36:04</t>
-  </si>
-  <si>
-    <t>23/10/2024 06:57:23</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:36:08</t>
-  </si>
-  <si>
-    <t>23/10/2024 06:57:44</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:36:57</t>
-  </si>
-  <si>
-    <t>23/10/2024 07:03:39</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:37:45</t>
-  </si>
-  <si>
-    <t>23/10/2024 07:03:40</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:38:25</t>
-  </si>
-  <si>
-    <t>23/10/2024 07:47:41</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:39:03</t>
-  </si>
-  <si>
-    <t>23/10/2024 07:49:07</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:39:48</t>
-  </si>
-  <si>
-    <t>23/10/2024 07:49:39</t>
-  </si>
-  <si>
-    <t>23/10/2024 07:49:48</t>
-  </si>
-  <si>
-    <t>pedro.lopez&amp;pineed</t>
-  </si>
-  <si>
-    <t>PILOTO</t>
-  </si>
-  <si>
-    <t>23/10/2024 07:55:08</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:44:48</t>
-  </si>
-  <si>
-    <t>23/10/2024 07:55:28</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:46:17</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:13:06</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:13:53</t>
-  </si>
-  <si>
-    <t>ana.martinez&amp;pineed</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:01:45</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:46:39</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:33:03</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:47:38</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:34:28</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:48:29</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:35:03</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:49:58</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:36:34</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:50:59</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:37:21</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:56:06</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:38:10</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:07:12</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:38:50</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:08:23</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:39:26</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:18:04</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:40:27</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:18:08</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:45:33</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:21:31</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:47:13</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:23:01</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:48:05</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:56:28</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:49:18</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:56:30</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:50:23</t>
-  </si>
-  <si>
-    <t>23/10/2024 10:06:58</t>
-  </si>
-  <si>
-    <t>23/10/2024 08:51:22</t>
-  </si>
-  <si>
-    <t>23/10/2024 10:16:03</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:06:57</t>
-  </si>
-  <si>
-    <t>23/10/2024 10:24:12</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:07:29</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:07:44</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:07:46</t>
-  </si>
-  <si>
-    <t>23/10/2024 10:25:11</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:08:42</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:09:35</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:10:23</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:12:20</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:13:58</t>
-  </si>
-  <si>
-    <t>23/10/2024 10:27:26</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:20:54</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:21:07</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>SECRETARIA</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:21:09</t>
-  </si>
-  <si>
-    <t>23/10/2024 10:46:02</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:34:22</t>
-  </si>
-  <si>
-    <t>23/10/2024 10:57:34</t>
-  </si>
-  <si>
-    <t>23/10/2024 09:50:36</t>
-  </si>
-  <si>
-    <t>23/10/2024 11:02:22</t>
-  </si>
-  <si>
-    <t>23/10/2024 10:13:51</t>
-  </si>
-  <si>
-    <t>23/10/2024 11:12:59</t>
-  </si>
-  <si>
-    <t>23/10/2024 10:23:06</t>
-  </si>
-  <si>
-    <t>23/10/2024 11:17:18</t>
-  </si>
-  <si>
     <t>23/10/2024 10:25:36</t>
   </si>
   <si>
-    <t/>
+    <t>23/10/2024 13:11:18</t>
   </si>
   <si>
     <t>23/10/2024 10:57:24</t>
   </si>
   <si>
+    <t>23/10/2024 13:16:33</t>
+  </si>
+  <si>
     <t>23/10/2024 11:01:10</t>
   </si>
   <si>
+    <t>23/10/2024 13:22:06</t>
+  </si>
+  <si>
     <t>23/10/2024 11:03:25</t>
   </si>
   <si>
+    <t>23/10/2024 13:25:26</t>
+  </si>
+  <si>
     <t>23/10/2024 11:13:15</t>
   </si>
   <si>
+    <t>23/10/2024 13:36:28</t>
+  </si>
+  <si>
     <t>23/10/2024 11:17:53</t>
   </si>
   <si>
+    <t>23/10/2024 13:37:17</t>
+  </si>
+  <si>
     <t>23/10/2024 11:17:54</t>
+  </si>
+  <si>
+    <t>23/10/2024 13:40:04</t>
+  </si>
+  <si>
+    <t>23/10/2024 12:47:16</t>
+  </si>
+  <si>
+    <t>23/10/2024 13:46:24</t>
+  </si>
+  <si>
+    <t>23/10/2024 13:14:20</t>
+  </si>
+  <si>
+    <t>23/10/2024 14:04:33</t>
+  </si>
+  <si>
+    <t>23/10/2024 13:20:28</t>
+  </si>
+  <si>
+    <t>23/10/2024 15:14:15</t>
+  </si>
+  <si>
+    <t>23/10/2024 13:22:20</t>
+  </si>
+  <si>
+    <t>23/10/2024 15:15:20</t>
+  </si>
+  <si>
+    <t>23/10/2024 13:32:37</t>
+  </si>
+  <si>
+    <t>23/10/2024 15:15:57</t>
+  </si>
+  <si>
+    <t>23/10/2024 13:36:37</t>
+  </si>
+  <si>
+    <t>23/10/2024 15:23:26</t>
+  </si>
+  <si>
+    <t>23/10/2024 13:39:55</t>
+  </si>
+  <si>
+    <t>23/10/2024 15:26:38</t>
+  </si>
+  <si>
+    <t>23/10/2024 13:40:58</t>
+  </si>
+  <si>
+    <t>23/10/2024 15:29:29</t>
+  </si>
+  <si>
+    <t>23/10/2024 14:00:38</t>
+  </si>
+  <si>
+    <t>23/10/2024 15:42:44</t>
+  </si>
+  <si>
+    <t>23/10/2024 15:13:11</t>
+  </si>
+  <si>
+    <t>23/10/2024 16:47:08</t>
+  </si>
+  <si>
+    <t>23/10/2024 15:14:37</t>
+  </si>
+  <si>
+    <t>23/10/2024 16:50:12</t>
+  </si>
+  <si>
+    <t>23/10/2024 15:15:44</t>
+  </si>
+  <si>
+    <t>23/10/2024 16:51:11</t>
+  </si>
+  <si>
+    <t>23/10/2024 15:19:13</t>
+  </si>
+  <si>
+    <t>23/10/2024 16:59:30</t>
+  </si>
+  <si>
+    <t>23/10/2024 15:23:42</t>
+  </si>
+  <si>
+    <t>23/10/2024 17:02:59</t>
+  </si>
+  <si>
+    <t>23/10/2024 15:27:07</t>
+  </si>
+  <si>
+    <t>23/10/2024 17:09:59</t>
+  </si>
+  <si>
+    <t>23/10/2024 15:42:35</t>
+  </si>
+  <si>
+    <t>23/10/2024 17:20:51</t>
+  </si>
+  <si>
+    <t>23/10/2024 16:46:31</t>
+  </si>
+  <si>
+    <t>23/10/2024 17:25:03</t>
+  </si>
+  <si>
+    <t>23/10/2024 16:49:33</t>
+  </si>
+  <si>
+    <t>23/10/2024 17:27:43</t>
+  </si>
+  <si>
+    <t>23/10/2024 16:50:22</t>
+  </si>
+  <si>
+    <t>23/10/2024 17:32:05</t>
+  </si>
+  <si>
+    <t>23/10/2024 18:47:42</t>
+  </si>
+  <si>
+    <t>23/10/2024 18:48:01</t>
+  </si>
+  <si>
+    <t>administrador.admin&amp;pineed</t>
   </si>
 </sst>
 </file>
@@ -2885,7 +3032,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D475"/>
+  <dimension ref="A1:D497"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -9431,10 +9578,10 @@
     </row>
     <row r="468">
       <c r="A468" t="s" s="1">
-        <v>236</v>
+        <v>934</v>
       </c>
       <c r="B468" t="s" s="1">
-        <v>237</v>
+        <v>935</v>
       </c>
       <c r="C468" t="s" s="0">
         <v>238</v>
@@ -9445,10 +9592,10 @@
     </row>
     <row r="469">
       <c r="A469" t="s" s="1">
-        <v>934</v>
-      </c>
-      <c r="B469" t="s" s="0">
-        <v>935</v>
+        <v>936</v>
+      </c>
+      <c r="B469" t="s" s="1">
+        <v>937</v>
       </c>
       <c r="C469" t="s" s="0">
         <v>238</v>
@@ -9459,10 +9606,10 @@
     </row>
     <row r="470">
       <c r="A470" t="s" s="1">
-        <v>936</v>
-      </c>
-      <c r="B470" t="s" s="0">
-        <v>935</v>
+        <v>938</v>
+      </c>
+      <c r="B470" t="s" s="1">
+        <v>939</v>
       </c>
       <c r="C470" t="s" s="0">
         <v>238</v>
@@ -9473,10 +9620,10 @@
     </row>
     <row r="471">
       <c r="A471" t="s" s="1">
-        <v>937</v>
-      </c>
-      <c r="B471" t="s" s="0">
-        <v>935</v>
+        <v>940</v>
+      </c>
+      <c r="B471" t="s" s="1">
+        <v>941</v>
       </c>
       <c r="C471" t="s" s="0">
         <v>238</v>
@@ -9487,10 +9634,10 @@
     </row>
     <row r="472">
       <c r="A472" t="s" s="1">
-        <v>938</v>
-      </c>
-      <c r="B472" t="s" s="0">
-        <v>935</v>
+        <v>942</v>
+      </c>
+      <c r="B472" t="s" s="1">
+        <v>943</v>
       </c>
       <c r="C472" t="s" s="0">
         <v>238</v>
@@ -9501,10 +9648,10 @@
     </row>
     <row r="473">
       <c r="A473" t="s" s="1">
-        <v>939</v>
-      </c>
-      <c r="B473" t="s" s="0">
-        <v>935</v>
+        <v>944</v>
+      </c>
+      <c r="B473" t="s" s="1">
+        <v>945</v>
       </c>
       <c r="C473" t="s" s="0">
         <v>238</v>
@@ -9515,10 +9662,10 @@
     </row>
     <row r="474">
       <c r="A474" t="s" s="1">
-        <v>940</v>
-      </c>
-      <c r="B474" t="s" s="0">
-        <v>935</v>
+        <v>946</v>
+      </c>
+      <c r="B474" t="s" s="1">
+        <v>947</v>
       </c>
       <c r="C474" t="s" s="0">
         <v>238</v>
@@ -9529,15 +9676,323 @@
     </row>
     <row r="475">
       <c r="A475" t="s" s="1">
-        <v>941</v>
-      </c>
-      <c r="B475" t="s" s="0">
-        <v>935</v>
+        <v>948</v>
+      </c>
+      <c r="B475" t="s" s="1">
+        <v>949</v>
       </c>
       <c r="C475" t="s" s="0">
         <v>238</v>
       </c>
       <c r="D475" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="s" s="1">
+        <v>950</v>
+      </c>
+      <c r="B476" t="s" s="1">
+        <v>951</v>
+      </c>
+      <c r="C476" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="D476" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="s" s="1">
+        <v>952</v>
+      </c>
+      <c r="B477" t="s" s="1">
+        <v>953</v>
+      </c>
+      <c r="C477" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="D477" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="s" s="1">
+        <v>954</v>
+      </c>
+      <c r="B478" t="s" s="1">
+        <v>955</v>
+      </c>
+      <c r="C478" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="D478" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="s" s="1">
+        <v>956</v>
+      </c>
+      <c r="B479" t="s" s="1">
+        <v>957</v>
+      </c>
+      <c r="C479" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="D479" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="s" s="1">
+        <v>958</v>
+      </c>
+      <c r="B480" t="s" s="1">
+        <v>959</v>
+      </c>
+      <c r="C480" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="D480" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="s" s="1">
+        <v>960</v>
+      </c>
+      <c r="B481" t="s" s="1">
+        <v>961</v>
+      </c>
+      <c r="C481" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="D481" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="s" s="1">
+        <v>962</v>
+      </c>
+      <c r="B482" t="s" s="1">
+        <v>963</v>
+      </c>
+      <c r="C482" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="D482" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="s" s="1">
+        <v>964</v>
+      </c>
+      <c r="B483" t="s" s="1">
+        <v>965</v>
+      </c>
+      <c r="C483" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="D483" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="s" s="1">
+        <v>966</v>
+      </c>
+      <c r="B484" t="s" s="1">
+        <v>967</v>
+      </c>
+      <c r="C484" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="D484" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="s" s="1">
+        <v>968</v>
+      </c>
+      <c r="B485" t="s" s="1">
+        <v>969</v>
+      </c>
+      <c r="C485" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="D485" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="s" s="1">
+        <v>970</v>
+      </c>
+      <c r="B486" t="s" s="1">
+        <v>971</v>
+      </c>
+      <c r="C486" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="D486" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="s" s="1">
+        <v>972</v>
+      </c>
+      <c r="B487" t="s" s="1">
+        <v>973</v>
+      </c>
+      <c r="C487" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="D487" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="s" s="1">
+        <v>974</v>
+      </c>
+      <c r="B488" t="s" s="1">
+        <v>975</v>
+      </c>
+      <c r="C488" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="D488" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="s" s="1">
+        <v>976</v>
+      </c>
+      <c r="B489" t="s" s="1">
+        <v>977</v>
+      </c>
+      <c r="C489" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="D489" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="s" s="1">
+        <v>978</v>
+      </c>
+      <c r="B490" t="s" s="1">
+        <v>979</v>
+      </c>
+      <c r="C490" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="D490" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="s" s="1">
+        <v>980</v>
+      </c>
+      <c r="B491" t="s" s="1">
+        <v>981</v>
+      </c>
+      <c r="C491" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="D491" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="s" s="1">
+        <v>982</v>
+      </c>
+      <c r="B492" t="s" s="1">
+        <v>983</v>
+      </c>
+      <c r="C492" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="D492" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="s" s="1">
+        <v>984</v>
+      </c>
+      <c r="B493" t="s" s="1">
+        <v>985</v>
+      </c>
+      <c r="C493" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="D493" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="s" s="1">
+        <v>986</v>
+      </c>
+      <c r="B494" t="s" s="1">
+        <v>987</v>
+      </c>
+      <c r="C494" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="D494" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="s" s="1">
+        <v>236</v>
+      </c>
+      <c r="B495" t="s" s="1">
+        <v>237</v>
+      </c>
+      <c r="C495" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="D495" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="s" s="1">
+        <v>988</v>
+      </c>
+      <c r="B496" t="s" s="1">
+        <v>989</v>
+      </c>
+      <c r="C496" t="s" s="0">
+        <v>990</v>
+      </c>
+      <c r="D496" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="s" s="1">
+        <v>988</v>
+      </c>
+      <c r="B497" t="s" s="1">
+        <v>989</v>
+      </c>
+      <c r="C497" t="s" s="0">
+        <v>990</v>
+      </c>
+      <c r="D497" t="s" s="0">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
solucion de interconexion que presentaba problemas
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/LOGGIN.xlsx
+++ b/ProyectoPooDist/excels/LOGGIN.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="122">
   <si>
     <t>Tiempo Entrada</t>
   </si>
@@ -258,6 +258,126 @@
   </si>
   <si>
     <t>26/10/2024 18:18:35</t>
+  </si>
+  <si>
+    <t>27/10/2024 10:04:28</t>
+  </si>
+  <si>
+    <t>27/10/2024 10:10:36</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>ADMINISTRADOR</t>
+  </si>
+  <si>
+    <t>27/10/2024 08:28:38</t>
+  </si>
+  <si>
+    <t>27/10/2024 08:28:53</t>
+  </si>
+  <si>
+    <t>27/10/2024 08:29:51</t>
+  </si>
+  <si>
+    <t>27/10/2024 08:30:06</t>
+  </si>
+  <si>
+    <t>27/10/2024 08:44:52</t>
+  </si>
+  <si>
+    <t>27/10/2024 08:45:34</t>
+  </si>
+  <si>
+    <t>27/10/2024 08:46:27</t>
+  </si>
+  <si>
+    <t>27/10/2024 08:47:56</t>
+  </si>
+  <si>
+    <t>27/10/2024 08:49:30</t>
+  </si>
+  <si>
+    <t>27/10/2024 08:50:59</t>
+  </si>
+  <si>
+    <t>27/10/2024 08:51:48</t>
+  </si>
+  <si>
+    <t>27/10/2024 08:52:07</t>
+  </si>
+  <si>
+    <t>27/10/2024 08:52:57</t>
+  </si>
+  <si>
+    <t>27/10/2024 08:55:57</t>
+  </si>
+  <si>
+    <t>27/10/2024 08:59:01</t>
+  </si>
+  <si>
+    <t>27/10/2024 08:59:19</t>
+  </si>
+  <si>
+    <t>27/10/2024 08:59:54</t>
+  </si>
+  <si>
+    <t>27/10/2024 09:01:43</t>
+  </si>
+  <si>
+    <t>27/10/2024 09:02:51</t>
+  </si>
+  <si>
+    <t>27/10/2024 09:03:08</t>
+  </si>
+  <si>
+    <t>27/10/2024 09:03:52</t>
+  </si>
+  <si>
+    <t>27/10/2024 09:06:44</t>
+  </si>
+  <si>
+    <t>27/10/2024 09:13:19</t>
+  </si>
+  <si>
+    <t>27/10/2024 09:13:58</t>
+  </si>
+  <si>
+    <t>27/10/2024 09:14:35</t>
+  </si>
+  <si>
+    <t>27/10/2024 09:18:29</t>
+  </si>
+  <si>
+    <t>27/10/2024 09:19:24</t>
+  </si>
+  <si>
+    <t>27/10/2024 09:21:12</t>
+  </si>
+  <si>
+    <t>27/10/2024 09:28:41</t>
+  </si>
+  <si>
+    <t>27/10/2024 09:31:49</t>
+  </si>
+  <si>
+    <t>27/10/2024 09:35:22</t>
+  </si>
+  <si>
+    <t>27/10/2024 09:37:30</t>
+  </si>
+  <si>
+    <t>27/10/2024 09:41:47</t>
+  </si>
+  <si>
+    <t>27/10/2024 09:45:29</t>
+  </si>
+  <si>
+    <t>27/10/2024 09:46:11</t>
+  </si>
+  <si>
+    <t>27/10/2024 09:46:55</t>
   </si>
 </sst>
 </file>
@@ -305,7 +425,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -871,6 +991,286 @@
         <v>69</v>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="s" s="1">
+        <v>82</v>
+      </c>
+      <c r="B41" t="s" s="1">
+        <v>83</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="D41" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="1">
+        <v>86</v>
+      </c>
+      <c r="B42" t="s" s="1">
+        <v>87</v>
+      </c>
+      <c r="C42" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="D42" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="1">
+        <v>88</v>
+      </c>
+      <c r="B43" t="s" s="1">
+        <v>89</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="D43" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="1">
+        <v>90</v>
+      </c>
+      <c r="B44" t="s" s="1">
+        <v>91</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="D44" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="1">
+        <v>92</v>
+      </c>
+      <c r="B45" t="s" s="1">
+        <v>93</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="D45" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="1">
+        <v>94</v>
+      </c>
+      <c r="B46" t="s" s="1">
+        <v>95</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="D46" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="B47" t="s" s="1">
+        <v>97</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="D47" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="1">
+        <v>98</v>
+      </c>
+      <c r="B48" t="s" s="1">
+        <v>99</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="D48" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="1">
+        <v>100</v>
+      </c>
+      <c r="B49" t="s" s="1">
+        <v>101</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="D49" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="1">
+        <v>102</v>
+      </c>
+      <c r="B50" t="s" s="1">
+        <v>103</v>
+      </c>
+      <c r="C50" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="D50" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="1">
+        <v>104</v>
+      </c>
+      <c r="B51" t="s" s="1">
+        <v>105</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="D51" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="1">
+        <v>106</v>
+      </c>
+      <c r="B52" t="s" s="1">
+        <v>107</v>
+      </c>
+      <c r="C52" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="D52" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="1">
+        <v>108</v>
+      </c>
+      <c r="B53" t="s" s="1">
+        <v>109</v>
+      </c>
+      <c r="C53" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="D53" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="1">
+        <v>110</v>
+      </c>
+      <c r="B54" t="s" s="1">
+        <v>111</v>
+      </c>
+      <c r="C54" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="D54" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="1">
+        <v>112</v>
+      </c>
+      <c r="B55" t="s" s="1">
+        <v>113</v>
+      </c>
+      <c r="C55" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="D55" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="1">
+        <v>114</v>
+      </c>
+      <c r="B56" t="s" s="1">
+        <v>115</v>
+      </c>
+      <c r="C56" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="D56" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="1">
+        <v>116</v>
+      </c>
+      <c r="B57" t="s" s="1">
+        <v>117</v>
+      </c>
+      <c r="C57" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="D57" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="1">
+        <v>118</v>
+      </c>
+      <c r="B58" t="s" s="1">
+        <v>119</v>
+      </c>
+      <c r="C58" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="D58" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="1">
+        <v>120</v>
+      </c>
+      <c r="B59" t="s" s="1">
+        <v>121</v>
+      </c>
+      <c r="C59" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="D59" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="1">
+        <v>82</v>
+      </c>
+      <c r="B60" t="s" s="1">
+        <v>83</v>
+      </c>
+      <c r="C60" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="D60" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>